<commit_message>
Com. 11/08/2025 #2: Detalles
</commit_message>
<xml_diff>
--- a/TAP Tema 1/results/try.xlsx
+++ b/TAP Tema 1/results/try.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>recordId</t>
   </si>
@@ -41,12 +41,24 @@
     <t>deleted</t>
   </si>
   <si>
+    <t>Rf7971</t>
+  </si>
+  <si>
+    <t>Udd529</t>
+  </si>
+  <si>
+    <t>Aguascalientes</t>
+  </si>
+  <si>
+    <t>Gastronomía</t>
+  </si>
+  <si>
+    <t>src/main/java/proyecto/resources/agus/489496123_1872564096894029_4907360869533054311_n.jpg</t>
+  </si>
+  <si>
     <t>R23387</t>
   </si>
   <si>
-    <t>Udd529</t>
-  </si>
-  <si>
     <t>Baja California</t>
   </si>
   <si>
@@ -62,6 +74,15 @@
     <t>src/main/java/proyecto/resources/baca/download.jpg</t>
   </si>
   <si>
+    <t>R56a72</t>
+  </si>
+  <si>
+    <t>Gastronomia BJ</t>
+  </si>
+  <si>
+    <t>src/main/java/proyecto/resources/baca/492522295_1240113004212486_7120062313825821510_n.jpg</t>
+  </si>
+  <si>
     <t>Rc35d7</t>
   </si>
   <si>
@@ -126,9 +147,6 @@
   </si>
   <si>
     <t>Puebla</t>
-  </si>
-  <si>
-    <t>Gastronomía</t>
   </si>
   <si>
     <t xml:space="preserve">Prueba de eliminacion </t>
@@ -182,7 +200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -234,13 +252,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>13</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>15</v>
       </c>
       <c r="I2" t="b" s="0">
         <v>0</v>
@@ -248,28 +266,28 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E3" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="E3" t="b" s="0">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="G3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="H3" t="s" s="0">
         <v>19</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>20</v>
       </c>
       <c r="I3" t="b" s="0">
         <v>0</v>
@@ -277,13 +295,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>12</v>
@@ -292,13 +310,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I4" t="b" s="0">
         <v>0</v>
@@ -306,28 +324,28 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E5" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="H5" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E5" t="b" s="0">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>30</v>
       </c>
       <c r="I5" t="b" s="0">
         <v>0</v>
@@ -335,28 +353,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E6" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="H6" t="s" s="0">
         <v>32</v>
-      </c>
-      <c r="E6" t="b" s="0">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>35</v>
       </c>
       <c r="I6" t="b" s="0">
         <v>0</v>
@@ -364,30 +382,88 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E7" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s" s="0">
+      <c r="H7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="I7" t="b" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="E7" t="b" s="0">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s" s="0">
+      <c r="B8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="G7" t="s" s="0">
+      <c r="E8" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="G8" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I7" t="b" s="0">
+      <c r="H8" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I8" t="b" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E9" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="I9" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Com. 11/08/2025 #4: 1. Funcionamiento de ventana de resumen funcional
</commit_message>
<xml_diff>
--- a/TAP Tema 1/results/try.xlsx
+++ b/TAP Tema 1/results/try.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>recordId</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>src/main/java/proyecto/resources/camp/555472471_776962455177966_3128049131977084705_n.jpg</t>
+  </si>
+  <si>
+    <t>Rc10d1</t>
+  </si>
+  <si>
+    <t>Chiapas</t>
+  </si>
+  <si>
+    <t>adasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>src/main/java/proyecto/resources/cdmx/495210901_122127526118410996_4349407357195817398_n.jpg</t>
   </si>
   <si>
     <t>R52ec2</t>
@@ -200,7 +215,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -443,7 +458,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>44</v>
@@ -452,7 +467,7 @@
         <v>12</v>
       </c>
       <c r="E9" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>45</v>
@@ -464,6 +479,35 @@
         <v>47</v>
       </c>
       <c r="I9" t="b" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E10" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="I10" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>